<commit_message>
19.01.2020 MC Sales Detais
</commit_message>
<xml_diff>
--- a/2020/January/All Details/19.01.2020/MC Balance Transfer Jan'2020.xlsx
+++ b/2020/January/All Details/19.01.2020/MC Balance Transfer Jan'2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\January\All Details\18.01.2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\January\All Details\19.01.2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1359E5-0098-468D-8EC2-F3569AF2835A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C7333C-971F-4B3C-B20B-0AB53F3FB2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,9 +304,6 @@
     <t>Atik</t>
   </si>
   <si>
-    <t>Desh Tel</t>
-  </si>
-  <si>
     <t>16.01.2020</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>Jafor Vai</t>
+  </si>
+  <si>
+    <t>19.01.2020</t>
   </si>
 </sst>
 </file>
@@ -1633,9 +1633,9 @@
   <dimension ref="A1:BI232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
+      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="19" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="2">
         <v>495290</v>
@@ -3044,7 +3044,7 @@
         <v>390</v>
       </c>
       <c r="J19" s="64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="19"/>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="20" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" s="2">
         <v>317910</v>
@@ -3124,7 +3124,7 @@
         <v>180</v>
       </c>
       <c r="J20" s="64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="19"/>
@@ -3179,21 +3179,33 @@
       <c r="BI20" s="7"/>
     </row>
     <row r="21" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="2">
+        <v>240825</v>
+      </c>
+      <c r="C21" s="2">
+        <v>276200</v>
+      </c>
+      <c r="D21" s="2">
+        <v>590</v>
+      </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>276790</v>
       </c>
       <c r="F21" s="135"/>
       <c r="G21" s="19"/>
       <c r="H21" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
+      <c r="I21" s="64">
+        <v>1200</v>
+      </c>
+      <c r="J21" s="64" t="s">
+        <v>88</v>
+      </c>
       <c r="K21" s="7"/>
       <c r="L21" s="19"/>
       <c r="M21" s="7"/>
@@ -4066,23 +4078,23 @@
       </c>
       <c r="B34" s="2">
         <f>SUM(B6:B33)</f>
-        <v>4683875</v>
+        <v>4924700</v>
       </c>
       <c r="C34" s="2">
         <f>SUM(C6:C33)</f>
-        <v>4635917</v>
+        <v>4912117</v>
       </c>
       <c r="D34" s="2">
         <f>SUM(D6:D33)</f>
-        <v>16652</v>
+        <v>17242</v>
       </c>
       <c r="E34" s="2">
         <f>SUM(E6:E33)</f>
-        <v>4652569</v>
+        <v>4929359</v>
       </c>
       <c r="F34" s="94">
         <f>B34-E34</f>
-        <v>31306</v>
+        <v>-4659</v>
       </c>
       <c r="G34" s="114"/>
       <c r="H34" s="124"/>
@@ -4631,10 +4643,10 @@
     </row>
     <row r="42" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C42" s="2">
         <v>11080</v>
@@ -4772,14 +4784,14 @@
     </row>
     <row r="44" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="2">
         <v>3000</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>12</v>
@@ -4847,7 +4859,7 @@
       <c r="A45" s="73"/>
       <c r="B45" s="74"/>
       <c r="C45" s="75">
-        <v>2234</v>
+        <v>4839</v>
       </c>
       <c r="D45" s="76"/>
       <c r="E45" s="3"/>
@@ -5176,10 +5188,10 @@
       </c>
       <c r="B50" s="43"/>
       <c r="C50" s="98">
-        <v>97800</v>
+        <v>98750</v>
       </c>
       <c r="D50" s="99" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="12"/>
@@ -5310,10 +5322,10 @@
       </c>
       <c r="B52" s="43"/>
       <c r="C52" s="98">
-        <v>356810</v>
+        <v>316810</v>
       </c>
       <c r="D52" s="99" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="43"/>
@@ -5379,10 +5391,10 @@
       </c>
       <c r="B53" s="43"/>
       <c r="C53" s="98">
-        <v>193250</v>
+        <v>196190</v>
       </c>
       <c r="D53" s="102" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="12"/>
@@ -5451,7 +5463,7 @@
         <v>24000</v>
       </c>
       <c r="D54" s="99" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="64"/>
@@ -5517,7 +5529,7 @@
       </c>
       <c r="B55" s="43"/>
       <c r="C55" s="98">
-        <v>12000</v>
+        <v>20040</v>
       </c>
       <c r="D55" s="102" t="s">
         <v>77</v>
@@ -5654,7 +5666,7 @@
         <v>43000</v>
       </c>
       <c r="D57" s="97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="43"/>
@@ -5720,10 +5732,10 @@
       </c>
       <c r="B58" s="43"/>
       <c r="C58" s="98">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="D58" s="107" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="43"/>
@@ -5789,10 +5801,10 @@
       </c>
       <c r="B59" s="43"/>
       <c r="C59" s="98">
-        <v>6000</v>
+        <v>5500</v>
       </c>
       <c r="D59" s="107" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="64"/>
@@ -5854,14 +5866,14 @@
     </row>
     <row r="60" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="100" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B60" s="43"/>
       <c r="C60" s="98">
         <v>32180</v>
       </c>
       <c r="D60" s="107" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="43"/>
@@ -5923,14 +5935,14 @@
     </row>
     <row r="61" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="105" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B61" s="43"/>
       <c r="C61" s="98">
         <v>10000</v>
       </c>
       <c r="D61" s="99" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="43"/>
@@ -5992,14 +6004,14 @@
     </row>
     <row r="62" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="100" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B62" s="43"/>
       <c r="C62" s="98">
         <v>6890</v>
       </c>
       <c r="D62" s="99" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="19"/>
@@ -6060,16 +6072,10 @@
       <c r="BI62" s="7"/>
     </row>
     <row r="63" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="100" t="s">
-        <v>79</v>
-      </c>
+      <c r="A63" s="100"/>
       <c r="B63" s="43"/>
-      <c r="C63" s="98">
-        <v>11000</v>
-      </c>
-      <c r="D63" s="99" t="s">
-        <v>80</v>
-      </c>
+      <c r="C63" s="98"/>
+      <c r="D63" s="99"/>
       <c r="E63" s="3"/>
       <c r="F63" s="160" t="s">
         <v>28</v>
@@ -6204,14 +6210,14 @@
     </row>
     <row r="65" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="105" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B65" s="43"/>
       <c r="C65" s="98">
         <v>1070</v>
       </c>
       <c r="D65" s="99" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="65"/>
@@ -8639,7 +8645,7 @@
       <c r="B99" s="159"/>
       <c r="C99" s="45">
         <f>SUM(C38:C98)</f>
-        <v>1509516</v>
+        <v>1473551</v>
       </c>
       <c r="D99" s="41"/>
       <c r="F99" s="23"/>
@@ -8774,7 +8780,7 @@
       <c r="B101" s="157"/>
       <c r="C101" s="42">
         <f>C99+L122</f>
-        <v>1509516</v>
+        <v>1473551</v>
       </c>
       <c r="D101" s="26"/>
       <c r="F101" s="24"/>

</xml_diff>